<commit_message>
Remove duplicates from different worksheets in excel
Remove duplicates from different worksheets in excel
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\RemoveDuplicatesActivityInExcel\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD231DE-E0CF-45A9-8B3D-6E285D97AAA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE701A15-9AB6-41C4-9C9F-80399EBB3D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>Yi Wong</t>
+  </si>
+  <si>
+    <t>row 2 and 16 are same</t>
+  </si>
+  <si>
+    <t>row 5-17, 7-19 and 12-18 are duplicate rows</t>
   </si>
 </sst>
 </file>
@@ -256,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -281,6 +287,8 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,24 +866,16 @@
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="7">
-        <v>19</v>
-      </c>
-      <c r="D16" s="7">
-        <v>19</v>
-      </c>
-      <c r="E16" s="7">
-        <v>20</v>
-      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
       <c r="F16" s="2"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G12">
@@ -888,10 +888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D0D904-0EFC-4A07-A959-2FE47D0AB604}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,16 +1167,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C15" s="10">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D15" s="10">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E15" s="10">
         <v>18</v>
@@ -1185,39 +1185,35 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C16" s="11">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D16" s="11">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E16" s="11">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="10">
-        <v>14</v>
-      </c>
-      <c r="D17" s="10">
-        <v>13</v>
-      </c>
-      <c r="E17" s="10">
-        <v>19</v>
-      </c>
-      <c r="F17" s="2"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="G18" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Remove duplicate column/row from worksheet in excel
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\RemoveDuplicatesActivityInExcel\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE701A15-9AB6-41C4-9C9F-80399EBB3D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A7A498-5490-4F9C-BA81-AE073C51F504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -571,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -890,7 +890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D0D904-0EFC-4A07-A959-2FE47D0AB604}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>

</xml_diff>